<commit_message>
Updating helsinki excell files by freezing Fajr and midnight
</commit_message>
<xml_diff>
--- a/adhan_excel/helsinki/4.xlsx
+++ b/adhan_excel/helsinki/4.xlsx
@@ -7,11 +7,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="v1ZMqrtmOcvXSxrMp8Pg4ojFLZUEh0NuBDKFH8IjXpw="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Päivämäärä
 تاریخ</t>
@@ -83,9 +88,6 @@
   </si>
   <si>
     <t>27/4</t>
-  </si>
-  <si>
-    <t>*</t>
   </si>
   <si>
     <t>28/4</t>
@@ -150,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -162,9 +164,6 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
@@ -424,11 +423,11 @@
       <c r="D2" s="3">
         <v>0.5583333333333333</v>
       </c>
-      <c r="E2" s="4">
-        <v>0.8368055555555556</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.8548611111111111</v>
+      <c r="E2" s="3">
+        <v>0.8354166666666667</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.8534722222222222</v>
       </c>
       <c r="G2" s="3">
         <v>0.010416666666666666</v>
@@ -438,20 +437,20 @@
       <c r="A3" s="2">
         <v>44596.0</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.18263888888888888</v>
+      <c r="B3" s="3">
+        <v>0.18194444444444444</v>
       </c>
       <c r="C3" s="3">
         <v>0.27847222222222223</v>
       </c>
-      <c r="D3" s="4">
-        <v>0.5583333333333333</v>
+      <c r="D3" s="3">
+        <v>0.5576388888888889</v>
       </c>
       <c r="E3" s="3">
-        <v>0.8388888888888889</v>
+        <v>0.8368055555555556</v>
       </c>
       <c r="F3" s="3">
-        <v>0.8569444444444444</v>
+        <v>0.8555555555555555</v>
       </c>
       <c r="G3" s="3">
         <v>0.009722222222222222</v>
@@ -471,10 +470,10 @@
         <v>0.5576388888888889</v>
       </c>
       <c r="E4" s="3">
-        <v>0.8402777777777778</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.8583333333333333</v>
+        <v>0.8388888888888889</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.8569444444444444</v>
       </c>
       <c r="G4" s="3">
         <v>0.009027777777777777</v>
@@ -493,11 +492,11 @@
       <c r="D5" s="3">
         <v>0.5576388888888889</v>
       </c>
-      <c r="E5" s="4">
-        <v>0.8416666666666667</v>
+      <c r="E5" s="3">
+        <v>0.8402777777777778</v>
       </c>
       <c r="F5" s="3">
-        <v>0.8604166666666667</v>
+        <v>0.8590277777777777</v>
       </c>
       <c r="G5" s="3">
         <v>0.008333333333333333</v>
@@ -507,20 +506,20 @@
       <c r="A6" s="2">
         <v>44685.0</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.1736111111111111</v>
+      <c r="B6" s="3">
+        <v>0.17291666666666666</v>
       </c>
       <c r="C6" s="3">
         <v>0.2722222222222222</v>
       </c>
-      <c r="D6" s="4">
-        <v>0.5576388888888889</v>
+      <c r="D6" s="3">
+        <v>0.5569444444444445</v>
       </c>
       <c r="E6" s="3">
-        <v>0.84375</v>
+        <v>0.8423611111111111</v>
       </c>
       <c r="F6" s="3">
-        <v>0.8625</v>
+        <v>0.8604166666666667</v>
       </c>
       <c r="G6" s="3">
         <v>0.007638888888888889</v>
@@ -536,14 +535,14 @@
       <c r="C7" s="3">
         <v>0.2701388888888889</v>
       </c>
-      <c r="D7" s="4">
-        <v>0.5576388888888889</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.8451388888888889</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.8638888888888889</v>
+      <c r="D7" s="3">
+        <v>0.5569444444444445</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.84375</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.8625</v>
       </c>
       <c r="G7" s="3">
         <v>0.006944444444444444</v>
@@ -563,10 +562,10 @@
         <v>0.5569444444444445</v>
       </c>
       <c r="E8" s="3">
-        <v>0.8472222222222222</v>
+        <v>0.8458333333333333</v>
       </c>
       <c r="F8" s="3">
-        <v>0.8659722222222223</v>
+        <v>0.8645833333333334</v>
       </c>
       <c r="G8" s="3">
         <v>0.00625</v>
@@ -585,11 +584,11 @@
       <c r="D9" s="3">
         <v>0.5569444444444445</v>
       </c>
-      <c r="E9" s="4">
-        <v>0.8486111111111111</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.8673611111111111</v>
+      <c r="E9" s="3">
+        <v>0.8472222222222222</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.8659722222222223</v>
       </c>
       <c r="G9" s="3">
         <v>0.005555555555555556</v>
@@ -605,14 +604,14 @@
       <c r="C10" s="3">
         <v>0.2638888888888889</v>
       </c>
-      <c r="D10" s="4">
-        <v>0.5569444444444445</v>
+      <c r="D10" s="3">
+        <v>0.55625</v>
       </c>
       <c r="E10" s="3">
-        <v>0.8506944444444444</v>
+        <v>0.8493055555555555</v>
       </c>
       <c r="F10" s="3">
-        <v>0.8694444444444445</v>
+        <v>0.8680555555555556</v>
       </c>
       <c r="G10" s="3">
         <v>0.004861111111111111</v>
@@ -631,11 +630,11 @@
       <c r="D11" s="3">
         <v>0.55625</v>
       </c>
-      <c r="E11" s="4">
-        <v>0.8520833333333333</v>
+      <c r="E11" s="3">
+        <v>0.8506944444444444</v>
       </c>
       <c r="F11" s="3">
-        <v>0.8715277777777778</v>
+        <v>0.8694444444444445</v>
       </c>
       <c r="G11" s="3">
         <v>0.004166666666666667</v>
@@ -688,7 +687,7 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="3">
@@ -711,7 +710,7 @@
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="3">
@@ -734,7 +733,7 @@
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="3">
@@ -757,7 +756,7 @@
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="3">
@@ -780,7 +779,7 @@
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="3">
@@ -803,7 +802,7 @@
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="3">
@@ -826,7 +825,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="3">
@@ -849,7 +848,7 @@
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="3">
@@ -872,7 +871,7 @@
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="3">
@@ -895,7 +894,7 @@
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="3">
@@ -918,7 +917,7 @@
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="3">
@@ -941,7 +940,7 @@
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="3">
@@ -964,7 +963,7 @@
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="3">
@@ -987,7 +986,7 @@
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B27" s="3">
@@ -1010,11 +1009,11 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>22</v>
+      <c r="B28" s="3">
+        <v>0.07361111111111111</v>
       </c>
       <c r="C28" s="3">
         <v>0.22708333333333333</v>
@@ -1033,11 +1032,11 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>22</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.07361111111111111</v>
       </c>
       <c r="C29" s="3">
         <v>0.225</v>
@@ -1056,11 +1055,11 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>22</v>
+      <c r="A30" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.07361111111111111</v>
       </c>
       <c r="C30" s="3">
         <v>0.22361111111111112</v>
@@ -1079,11 +1078,11 @@
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>22</v>
+      <c r="A31" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.07361111111111111</v>
       </c>
       <c r="C31" s="3">
         <v>0.22152777777777777</v>

</xml_diff>